<commit_message>
Implement locale share message
</commit_message>
<xml_diff>
--- a/assets/names/female.xlsx
+++ b/assets/names/female.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Magic\crystal\assets\names\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65796DC-291F-44FF-A0C6-AB1BBA0CBF4F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205F617F-4A9B-4C58-BFBA-207730C7DD3A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{2D183772-4471-4E1B-B005-E87E8F4BFE26}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Grace</t>
+  </si>
+  <si>
+    <t>Powerful, creative, and determined. People named Chloe have a deep inner desire for a stable, loving family or community, and a need to work with others and to be appreciated.</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +492,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>

</xml_diff>